<commit_message>
Added question to QandA
</commit_message>
<xml_diff>
--- a/QandA DCC ELAN.xlsx
+++ b/QandA DCC ELAN.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{153D96DE-31FA-4330-AD97-4FFFCF4833B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\org\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BECC68-3DF4-4616-AD77-1D7FCC269B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Q&amp;A DCC ELAN </t>
   </si>
@@ -94,13 +99,16 @@
   </si>
   <si>
     <t>Is it possible to add general statistics on the unlinkable population per data upload, to aid in assessing differences within confounding variables and groups?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How much do the medication entries in ELAN GP differ from medication entries in Vektis? In theory they should be identical, but a lot of medication entries are missing in ELAN GP, for a large part this happens when the medication is prescribed by a specialist and this is not communicated to the GP His. I'm mainly interested in the medications commonly used for rheumatic diseases and prescribed by the specialists, to be precise the following level-4 ATC codes: A07EA, A07EC, H02AB, L01AA, L01BA, L01XC, L04AA, L04AB, L04AC, L04AD, L04AX, M01CB, M01CC, P01BA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,7 +310,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -616,28 +624,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="125.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="125.33203125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.75" customHeight="1">
+    <row r="1" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="24" customHeight="1">
+    <row r="2" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -645,295 +653,297 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19.5" customHeight="1">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1">
+    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" ht="29.25" customHeight="1">
+    <row r="8" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1">
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" ht="11.25" customHeight="1">
+    <row r="10" spans="1:2" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" ht="14.25" customHeight="1">
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" ht="13.5" customHeight="1">
+    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
+    <row r="13" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
+    <row r="14" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="24">
+    <row r="16" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="24">
+    <row r="17" spans="1:1" ht="27" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="24">
+    <row r="18" spans="1:1" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="24">
+    <row r="19" spans="1:1" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="24">
+    <row r="20" spans="1:1" ht="27" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:1">
+    <row r="21" spans="1:1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="12"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="12"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="12"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="12"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="12"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="12"/>
     </row>
   </sheetData>

</xml_diff>